<commit_message>
Excel tutorial: Count and countifs added
</commit_message>
<xml_diff>
--- a/excelIntro/Excel_Workshop.xlsx
+++ b/excelIntro/Excel_Workshop.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D635400-A2DD-1D4E-9A63-9352553EDB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="705" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22260" windowHeight="12640" tabRatio="705" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulas" sheetId="5" r:id="rId1"/>
@@ -18,17 +19,28 @@
     <sheet name="averageifs" sheetId="9" r:id="rId9"/>
     <sheet name="Final exercise" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="58">
   <si>
     <t>Participant</t>
   </si>
@@ -184,12 +196,30 @@
   </si>
   <si>
     <t>stdev</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Phones</t>
+  </si>
+  <si>
+    <t>No Phones</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Females</t>
+  </si>
+  <si>
+    <t>Males</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,7 +245,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -260,30 +290,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,19 +645,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -583,7 +665,7 @@
         <v>10.234</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -591,13 +673,13 @@
         <v>23.135999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -605,7 +687,7 @@
         <v>23.141400000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -613,20 +695,20 @@
         <v>35.2121</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -634,7 +716,7 @@
         <v>34.231999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -642,7 +724,7 @@
         <v>50.564999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -650,7 +732,7 @@
         <v>5.3639999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -658,7 +740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -670,22 +752,22 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -702,7 +784,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -717,7 +799,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -731,12 +813,12 @@
         <v>17</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -753,14 +835,14 @@
       <c r="H4" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -774,13 +856,13 @@
         <v>17</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -794,13 +876,13 @@
         <v>16</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -814,13 +896,13 @@
         <v>17</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -834,13 +916,13 @@
         <v>16</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -854,13 +936,13 @@
         <v>17</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -875,7 +957,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -889,13 +971,13 @@
         <v>17</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="3" t="s">
         <v>50</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -909,13 +991,13 @@
         <v>16</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="8"/>
+      <c r="I12" s="5"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -930,7 +1012,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -945,7 +1027,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -960,7 +1042,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -975,7 +1057,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -990,7 +1072,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1005,7 +1087,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1020,7 +1102,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1035,7 +1117,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1050,7 +1132,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1065,7 +1147,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1080,7 +1162,7 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1095,7 +1177,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1110,7 +1192,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1125,7 +1207,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1140,7 +1222,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1155,7 +1237,7 @@
       </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1170,7 +1252,7 @@
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1185,7 +1267,7 @@
       </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1210,23 +1292,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1258,7 +1340,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1276,7 +1358,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1294,7 +1376,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1308,7 +1390,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1322,7 +1404,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1336,7 +1418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1349,8 +1431,20 @@
       <c r="D8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1363,8 +1457,14 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1377,8 +1477,14 @@
       <c r="D10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1398,23 +1504,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1428,7 +1534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1446,7 +1552,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1464,7 +1570,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1482,7 +1588,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1496,7 +1602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1510,7 +1616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1524,7 +1630,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1538,7 +1644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1552,7 +1658,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1566,7 +1672,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1586,23 +1692,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1616,7 +1722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1634,7 +1740,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1652,7 +1758,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1670,7 +1776,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1684,7 +1790,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1702,7 +1808,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1720,7 +1826,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1738,7 +1844,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1752,7 +1858,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1770,7 +1876,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1788,7 +1894,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H12" t="s">
         <v>26</v>
       </c>
@@ -1800,23 +1906,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1830,7 +1936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1848,7 +1954,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1866,7 +1972,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1884,7 +1990,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1898,7 +2004,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1912,7 +2018,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1926,7 +2032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1940,7 +2046,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1954,7 +2060,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1968,7 +2074,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1988,21 +2094,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2022,7 +2128,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2038,7 +2144,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2054,7 +2160,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2070,7 +2176,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2086,7 +2192,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2102,7 +2208,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2118,7 +2224,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2134,7 +2240,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2150,7 +2256,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2166,7 +2272,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2188,21 +2294,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2222,7 +2328,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2244,7 +2350,7 @@
         <v>1937.4815971048449</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2260,7 +2366,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2276,7 +2382,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2292,7 +2398,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2308,7 +2414,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2330,7 +2436,7 @@
         <v>157.05187347257322</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2344,9 +2450,9 @@
         <v>17</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2362,7 +2468,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2378,7 +2484,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2400,19 +2506,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2432,7 +2538,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2446,7 +2552,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2460,7 +2566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2474,7 +2580,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2488,7 +2594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2502,7 +2608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2516,7 +2622,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2530,7 +2636,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2544,7 +2650,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2558,7 +2664,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2578,23 +2684,23 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2611,7 +2717,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2628,7 +2734,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2645,7 +2751,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2659,7 +2765,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2673,7 +2779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2686,12 +2792,12 @@
       <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2711,7 +2817,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2728,7 +2834,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2745,7 +2851,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2759,7 +2865,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>

</xml_diff>